<commit_message>
#16: Fixed configuration data mask alternate lines option.
</commit_message>
<xml_diff>
--- a/MapeamentoID_OP.xlsx
+++ b/MapeamentoID_OP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="833" firstSheet="1" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="833" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="ID'S" sheetId="1" r:id="rId1"/>
@@ -13873,6 +13873,27 @@
   </cellStyles>
   <dxfs count="293">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -13922,11 +13943,140 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -14049,6 +14199,250 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -14317,11 +14711,176 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -14408,11 +14967,231 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -14485,799 +15264,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -15326,6 +15312,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -15362,66 +15362,66 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabela12" displayName="Tabela12" ref="A1:K16" totalsRowShown="0" headerRowDxfId="236" dataDxfId="235">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabela12" displayName="Tabela12" ref="A1:K16" totalsRowShown="0" headerRowDxfId="199" dataDxfId="198">
   <autoFilter ref="A1:K16"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="ID" dataDxfId="234"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="233"/>
-    <tableColumn id="3" name="BACK COLOUR" dataDxfId="232"/>
-    <tableColumn id="4" name="KEY CODE" dataDxfId="231"/>
-    <tableColumn id="5" name="N° OBJETOS" dataDxfId="230"/>
-    <tableColumn id="6" name="N° MACROS" dataDxfId="229"/>
-    <tableColumn id="7" name="OBJ + POS" dataDxfId="228"/>
-    <tableColumn id="8" name="Colunas1" dataDxfId="227"/>
-    <tableColumn id="9" name="EVENT + MACRO ID" dataDxfId="226"/>
-    <tableColumn id="10" name="Colunas2" dataDxfId="225"/>
-    <tableColumn id="11" name="DESCRIÇÃO" dataDxfId="224"/>
+    <tableColumn id="1" name="ID" dataDxfId="197"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="196"/>
+    <tableColumn id="3" name="BACK COLOUR" dataDxfId="195"/>
+    <tableColumn id="4" name="KEY CODE" dataDxfId="194"/>
+    <tableColumn id="5" name="N° OBJETOS" dataDxfId="193"/>
+    <tableColumn id="6" name="N° MACROS" dataDxfId="192"/>
+    <tableColumn id="7" name="OBJ + POS" dataDxfId="191"/>
+    <tableColumn id="8" name="Colunas1" dataDxfId="190"/>
+    <tableColumn id="9" name="EVENT + MACRO ID" dataDxfId="189"/>
+    <tableColumn id="10" name="Colunas2" dataDxfId="188"/>
+    <tableColumn id="11" name="DESCRIÇÃO" dataDxfId="187"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:M135" totalsRowShown="0" headerRowDxfId="223">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:M135" totalsRowShown="0" headerRowDxfId="178">
   <autoFilter ref="A1:M135"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="ID" dataDxfId="222"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="221"/>
-    <tableColumn id="3" name="WIDTH" dataDxfId="220"/>
-    <tableColumn id="4" name="HEIGHT" dataDxfId="219"/>
-    <tableColumn id="5" name="HIDDEN" dataDxfId="218"/>
-    <tableColumn id="6" name="QTDE OBJETOS" dataDxfId="217"/>
-    <tableColumn id="7" name="QTDE MACROS" dataDxfId="216"/>
-    <tableColumn id="8" name="OBJ + POS" dataDxfId="215"/>
-    <tableColumn id="9" name="Colunas1" dataDxfId="214"/>
+    <tableColumn id="1" name="ID" dataDxfId="177"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="176"/>
+    <tableColumn id="3" name="WIDTH" dataDxfId="175"/>
+    <tableColumn id="4" name="HEIGHT" dataDxfId="174"/>
+    <tableColumn id="5" name="HIDDEN" dataDxfId="173"/>
+    <tableColumn id="6" name="QTDE OBJETOS" dataDxfId="172"/>
+    <tableColumn id="7" name="QTDE MACROS" dataDxfId="171"/>
+    <tableColumn id="8" name="OBJ + POS" dataDxfId="170"/>
+    <tableColumn id="9" name="Colunas1" dataDxfId="169"/>
     <tableColumn id="10" name="EVENT + MACRO ID"/>
-    <tableColumn id="11" name="Colunas2" dataDxfId="213"/>
-    <tableColumn id="12" name="DESCRIÇÃO" dataDxfId="212"/>
-    <tableColumn id="13" name="Colunas3" dataDxfId="211"/>
+    <tableColumn id="11" name="Colunas2" dataDxfId="168"/>
+    <tableColumn id="12" name="DESCRIÇÃO" dataDxfId="167"/>
+    <tableColumn id="13" name="Colunas3" dataDxfId="166"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:O58" totalsRowShown="0" headerRowDxfId="210">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:O58" totalsRowShown="0" headerRowDxfId="127">
   <autoFilter ref="A1:O58"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="ID" dataDxfId="209"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="208"/>
-    <tableColumn id="3" name="WIDTH" dataDxfId="207"/>
-    <tableColumn id="4" name="HEIGHT" dataDxfId="206"/>
-    <tableColumn id="5" name="BACK COLOUR" dataDxfId="205"/>
-    <tableColumn id="6" name="BORDER COLOUR" dataDxfId="204"/>
-    <tableColumn id="7" name="KEY CODE" dataDxfId="203"/>
-    <tableColumn id="8" name="OPTIONS" dataDxfId="202"/>
-    <tableColumn id="9" name="QTDE OBJETOS" dataDxfId="201"/>
-    <tableColumn id="10" name="QTDE MACROS" dataDxfId="200"/>
-    <tableColumn id="11" name="OBJ + POS" dataDxfId="199"/>
-    <tableColumn id="12" name="Colunas1" dataDxfId="198"/>
-    <tableColumn id="13" name="EVENT + MACRO ID" dataDxfId="197"/>
-    <tableColumn id="14" name="Colunas2" dataDxfId="196"/>
-    <tableColumn id="15" name="DESCRIÇÃO" dataDxfId="195"/>
+    <tableColumn id="1" name="ID" dataDxfId="126"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="125"/>
+    <tableColumn id="3" name="WIDTH" dataDxfId="124"/>
+    <tableColumn id="4" name="HEIGHT" dataDxfId="123"/>
+    <tableColumn id="5" name="BACK COLOUR" dataDxfId="122"/>
+    <tableColumn id="6" name="BORDER COLOUR" dataDxfId="121"/>
+    <tableColumn id="7" name="KEY CODE" dataDxfId="120"/>
+    <tableColumn id="8" name="OPTIONS" dataDxfId="119"/>
+    <tableColumn id="9" name="QTDE OBJETOS" dataDxfId="118"/>
+    <tableColumn id="10" name="QTDE MACROS" dataDxfId="117"/>
+    <tableColumn id="11" name="OBJ + POS" dataDxfId="116"/>
+    <tableColumn id="12" name="Colunas1" dataDxfId="115"/>
+    <tableColumn id="13" name="EVENT + MACRO ID" dataDxfId="114"/>
+    <tableColumn id="14" name="Colunas2" dataDxfId="113"/>
+    <tableColumn id="15" name="DESCRIÇÃO" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -15441,7 +15441,7 @@
     <tableColumn id="8" name="ENABLED"/>
     <tableColumn id="9" name="N° MACROS"/>
     <tableColumn id="10" name="EVENT + MACRO ID"/>
-    <tableColumn id="13" name="Colunas2" dataDxfId="194"/>
+    <tableColumn id="13" name="Colunas2" dataDxfId="110"/>
     <tableColumn id="11" name="DESCRIÇÃO"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -15449,23 +15449,23 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:N7" totalsRowShown="0" headerRowDxfId="193">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A1:N7" totalsRowShown="0" headerRowDxfId="108">
   <autoFilter ref="A1:N7"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="ID" dataDxfId="192"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="191"/>
-    <tableColumn id="3" name="WIDTH" dataDxfId="190"/>
-    <tableColumn id="4" name="HEIGHT" dataDxfId="189"/>
-    <tableColumn id="5" name="VARIABLE REF" dataDxfId="188"/>
-    <tableColumn id="6" name="VALUE" dataDxfId="187"/>
-    <tableColumn id="7" name="QTDE ITENS" dataDxfId="186"/>
-    <tableColumn id="8" name="OPTIONS" dataDxfId="185"/>
-    <tableColumn id="9" name="QTDE MACRO" dataDxfId="184"/>
-    <tableColumn id="10" name="OBJETO ID" dataDxfId="183"/>
-    <tableColumn id="11" name="Colunas1" dataDxfId="182"/>
-    <tableColumn id="12" name="EVENT + MACRO ID" dataDxfId="181"/>
-    <tableColumn id="13" name="Colunas2" dataDxfId="180"/>
-    <tableColumn id="14" name="DESCRIÇÃO" dataDxfId="179"/>
+    <tableColumn id="1" name="ID" dataDxfId="107"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="106"/>
+    <tableColumn id="3" name="WIDTH" dataDxfId="105"/>
+    <tableColumn id="4" name="HEIGHT" dataDxfId="104"/>
+    <tableColumn id="5" name="VARIABLE REF" dataDxfId="103"/>
+    <tableColumn id="6" name="VALUE" dataDxfId="102"/>
+    <tableColumn id="7" name="QTDE ITENS" dataDxfId="101"/>
+    <tableColumn id="8" name="OPTIONS" dataDxfId="100"/>
+    <tableColumn id="9" name="QTDE MACRO" dataDxfId="99"/>
+    <tableColumn id="10" name="OBJETO ID" dataDxfId="98"/>
+    <tableColumn id="11" name="Colunas1" dataDxfId="97"/>
+    <tableColumn id="12" name="EVENT + MACRO ID" dataDxfId="96"/>
+    <tableColumn id="13" name="Colunas2" dataDxfId="95"/>
+    <tableColumn id="14" name="DESCRIÇÃO" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -15475,27 +15475,27 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A1:U11" totalsRowShown="0">
   <autoFilter ref="A1:U11"/>
   <tableColumns count="21">
-    <tableColumn id="1" name="ID" dataDxfId="178"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="177"/>
-    <tableColumn id="3" name="WIDTH" dataDxfId="176"/>
-    <tableColumn id="4" name="HEIGHT" dataDxfId="175"/>
-    <tableColumn id="5" name="BACK COLOUR" dataDxfId="174"/>
-    <tableColumn id="6" name="FONT" dataDxfId="173"/>
-    <tableColumn id="7" name="OPTIONS" dataDxfId="172"/>
-    <tableColumn id="8" name="VARIABLE REF" dataDxfId="171"/>
-    <tableColumn id="9" name="VALUE" dataDxfId="170"/>
-    <tableColumn id="10" name="VALOR MÍNIMO" dataDxfId="169"/>
-    <tableColumn id="11" name="VALOR MÁXIMO" dataDxfId="168"/>
-    <tableColumn id="12" name="OFFSET" dataDxfId="167"/>
-    <tableColumn id="13" name="SCALE" dataDxfId="166"/>
-    <tableColumn id="14" name="N° DECIMAIS" dataDxfId="165"/>
-    <tableColumn id="15" name="FORMAT" dataDxfId="164"/>
-    <tableColumn id="16" name="JUSTIFICATION" dataDxfId="163"/>
-    <tableColumn id="17" name="OPTIONS 2" dataDxfId="162"/>
-    <tableColumn id="18" name="N° MACROS" dataDxfId="161"/>
+    <tableColumn id="1" name="ID" dataDxfId="92"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="91"/>
+    <tableColumn id="3" name="WIDTH" dataDxfId="90"/>
+    <tableColumn id="4" name="HEIGHT" dataDxfId="89"/>
+    <tableColumn id="5" name="BACK COLOUR" dataDxfId="88"/>
+    <tableColumn id="6" name="FONT" dataDxfId="87"/>
+    <tableColumn id="7" name="OPTIONS" dataDxfId="86"/>
+    <tableColumn id="8" name="VARIABLE REF" dataDxfId="85"/>
+    <tableColumn id="9" name="VALUE" dataDxfId="84"/>
+    <tableColumn id="10" name="VALOR MÍNIMO" dataDxfId="83"/>
+    <tableColumn id="11" name="VALOR MÁXIMO" dataDxfId="82"/>
+    <tableColumn id="12" name="OFFSET" dataDxfId="81"/>
+    <tableColumn id="13" name="SCALE" dataDxfId="80"/>
+    <tableColumn id="14" name="N° DECIMAIS" dataDxfId="79"/>
+    <tableColumn id="15" name="FORMAT" dataDxfId="78"/>
+    <tableColumn id="16" name="JUSTIFICATION" dataDxfId="77"/>
+    <tableColumn id="17" name="OPTIONS 2" dataDxfId="76"/>
+    <tableColumn id="18" name="N° MACROS" dataDxfId="75"/>
     <tableColumn id="19" name="EVENT + MACRO ID"/>
-    <tableColumn id="21" name="Colunas1" dataDxfId="160"/>
-    <tableColumn id="20" name="DESCRIÇÃO" dataDxfId="159"/>
+    <tableColumn id="21" name="Colunas1" dataDxfId="74"/>
+    <tableColumn id="20" name="DESCRIÇÃO" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -15547,7 +15547,7 @@
     <tableColumn id="14" name="TARGET VALUE"/>
     <tableColumn id="15" name="N° MACRO"/>
     <tableColumn id="16" name="EVENT + MACRO ID"/>
-    <tableColumn id="19" name="Colunas2" dataDxfId="158"/>
+    <tableColumn id="19" name="Colunas2" dataDxfId="71"/>
     <tableColumn id="17" name="DESCRIÇÃO"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -15555,7 +15555,7 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A1:D483" totalsRowShown="0" headerRowDxfId="157">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A1:D483" totalsRowShown="0" headerRowDxfId="70">
   <autoFilter ref="A1:D483"/>
   <tableColumns count="4">
     <tableColumn id="1" name="ID"/>
@@ -15568,45 +15568,45 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:N296" totalsRowShown="0" headerRowDxfId="156">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:N296" totalsRowShown="0" headerRowDxfId="53">
   <tableColumns count="14">
-    <tableColumn id="1" name="ID" dataDxfId="155"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="154"/>
+    <tableColumn id="1" name="ID" dataDxfId="52"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="51"/>
     <tableColumn id="3" name="WIDTH"/>
     <tableColumn id="4" name="HEIGHT"/>
-    <tableColumn id="5" name="BACK COLOUR" dataDxfId="153"/>
-    <tableColumn id="6" name="FONT" dataDxfId="152"/>
-    <tableColumn id="7" name="OPTIONS" dataDxfId="151"/>
-    <tableColumn id="8" name="VARIABLE REF" dataDxfId="150"/>
-    <tableColumn id="9" name="JUSTIFICATION" dataDxfId="149"/>
+    <tableColumn id="5" name="BACK COLOUR" dataDxfId="50"/>
+    <tableColumn id="6" name="FONT" dataDxfId="49"/>
+    <tableColumn id="7" name="OPTIONS" dataDxfId="48"/>
+    <tableColumn id="8" name="VARIABLE REF" dataDxfId="47"/>
+    <tableColumn id="9" name="JUSTIFICATION" dataDxfId="46"/>
     <tableColumn id="10" name="LENGTH"/>
-    <tableColumn id="11" name="VALUE" dataDxfId="148"/>
-    <tableColumn id="12" name="Colunas1" dataDxfId="147"/>
-    <tableColumn id="13" name="QTDE MACROS" dataDxfId="146"/>
-    <tableColumn id="14" name="DESCRIÇÃO" dataDxfId="145"/>
+    <tableColumn id="11" name="VALUE" dataDxfId="45"/>
+    <tableColumn id="12" name="Colunas1" dataDxfId="44"/>
+    <tableColumn id="13" name="QTDE MACROS" dataDxfId="43"/>
+    <tableColumn id="14" name="DESCRIÇÃO" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabela9" displayName="Tabela9" ref="A1:N2" totalsRowShown="0" headerRowDxfId="288" dataDxfId="287">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabela9" displayName="Tabela9" ref="A1:N2" totalsRowShown="0" headerRowDxfId="286" dataDxfId="285">
   <autoFilter ref="A1:N2"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="ID" dataDxfId="286"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="285"/>
-    <tableColumn id="3" name="BACK COLOUR" dataDxfId="284"/>
-    <tableColumn id="4" name="SELECTABLE" dataDxfId="283"/>
-    <tableColumn id="5" name="ACTIVE MASK" dataDxfId="282"/>
-    <tableColumn id="6" name="N° OBJETOS" dataDxfId="281"/>
-    <tableColumn id="7" name="N° MACROS" dataDxfId="280"/>
-    <tableColumn id="8" name="N° LANGUAGES" dataDxfId="279"/>
-    <tableColumn id="9" name="OBJ + POS" dataDxfId="278"/>
-    <tableColumn id="10" name="Colunas1" dataDxfId="277"/>
-    <tableColumn id="11" name="EVENT + MACRO ID" dataDxfId="276"/>
-    <tableColumn id="12" name="Colunas2" dataDxfId="275"/>
-    <tableColumn id="13" name="LANGUAGE CODE" dataDxfId="274"/>
-    <tableColumn id="14" name="DESCRIÇÃO" dataDxfId="273"/>
+    <tableColumn id="1" name="ID" dataDxfId="284"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="283"/>
+    <tableColumn id="3" name="BACK COLOUR" dataDxfId="282"/>
+    <tableColumn id="4" name="SELECTABLE" dataDxfId="281"/>
+    <tableColumn id="5" name="ACTIVE MASK" dataDxfId="280"/>
+    <tableColumn id="6" name="N° OBJETOS" dataDxfId="279"/>
+    <tableColumn id="7" name="N° MACROS" dataDxfId="278"/>
+    <tableColumn id="8" name="N° LANGUAGES" dataDxfId="277"/>
+    <tableColumn id="9" name="OBJ + POS" dataDxfId="276"/>
+    <tableColumn id="10" name="Colunas1" dataDxfId="275"/>
+    <tableColumn id="11" name="EVENT + MACRO ID" dataDxfId="274"/>
+    <tableColumn id="12" name="Colunas2" dataDxfId="273"/>
+    <tableColumn id="13" name="LANGUAGE CODE" dataDxfId="272"/>
+    <tableColumn id="14" name="DESCRIÇÃO" dataDxfId="271"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -15627,23 +15627,23 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tabela21" displayName="Tabela21" ref="A1:N2" totalsRowShown="0" dataDxfId="144">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tabela21" displayName="Tabela21" ref="A1:N2" totalsRowShown="0" dataDxfId="41">
   <autoFilter ref="A1:N2"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="ID" dataDxfId="143"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="142"/>
-    <tableColumn id="3" name="WIDTH" dataDxfId="141"/>
-    <tableColumn id="4" name="ACTUAL WIDHT" dataDxfId="140"/>
-    <tableColumn id="5" name="ACTUAL HEIGHT" dataDxfId="139"/>
-    <tableColumn id="6" name="FORMAT" dataDxfId="138"/>
-    <tableColumn id="7" name="OPTIONS" dataDxfId="137"/>
-    <tableColumn id="8" name="TRANSP. COLOUR" dataDxfId="136"/>
-    <tableColumn id="9" name="N° BYTES RAW DATA" dataDxfId="135"/>
-    <tableColumn id="10" name="N° MACRO" dataDxfId="134"/>
-    <tableColumn id="11" name="RAW DATA" dataDxfId="133"/>
-    <tableColumn id="12" name="EVENT + MACRO ID" dataDxfId="132"/>
-    <tableColumn id="13" name="DESCRIÇÃO" dataDxfId="131"/>
-    <tableColumn id="14" name="OBSERVAÇÃO" dataDxfId="130"/>
+    <tableColumn id="1" name="ID" dataDxfId="40"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="39"/>
+    <tableColumn id="3" name="WIDTH" dataDxfId="38"/>
+    <tableColumn id="4" name="ACTUAL WIDHT" dataDxfId="37"/>
+    <tableColumn id="5" name="ACTUAL HEIGHT" dataDxfId="36"/>
+    <tableColumn id="6" name="FORMAT" dataDxfId="35"/>
+    <tableColumn id="7" name="OPTIONS" dataDxfId="34"/>
+    <tableColumn id="8" name="TRANSP. COLOUR" dataDxfId="33"/>
+    <tableColumn id="9" name="N° BYTES RAW DATA" dataDxfId="32"/>
+    <tableColumn id="10" name="N° MACRO" dataDxfId="31"/>
+    <tableColumn id="11" name="RAW DATA" dataDxfId="30"/>
+    <tableColumn id="12" name="EVENT + MACRO ID" dataDxfId="29"/>
+    <tableColumn id="13" name="DESCRIÇÃO" dataDxfId="28"/>
+    <tableColumn id="14" name="OBSERVAÇÃO" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -15663,83 +15663,83 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela8" displayName="Tabela8" ref="A1:J12" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela8" displayName="Tabela8" ref="A1:J12" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:J12"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="ID" dataDxfId="127"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="126"/>
-    <tableColumn id="3" name="COLOUR" dataDxfId="125"/>
-    <tableColumn id="4" name="SIZE" dataDxfId="124"/>
-    <tableColumn id="5" name="FONT TYPE" dataDxfId="123"/>
-    <tableColumn id="6" name="STYLE" dataDxfId="122"/>
-    <tableColumn id="7" name="N° MACROS" dataDxfId="121"/>
-    <tableColumn id="8" name="EVENT + MACRO ID" dataDxfId="120"/>
-    <tableColumn id="11" name="Colunas2" dataDxfId="119"/>
-    <tableColumn id="9" name="DESCRIÇÃO" dataDxfId="118"/>
+    <tableColumn id="1" name="ID" dataDxfId="23"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="22"/>
+    <tableColumn id="3" name="COLOUR" dataDxfId="21"/>
+    <tableColumn id="4" name="SIZE" dataDxfId="20"/>
+    <tableColumn id="5" name="FONT TYPE" dataDxfId="19"/>
+    <tableColumn id="6" name="STYLE" dataDxfId="18"/>
+    <tableColumn id="7" name="N° MACROS" dataDxfId="17"/>
+    <tableColumn id="8" name="EVENT + MACRO ID" dataDxfId="16"/>
+    <tableColumn id="11" name="Colunas2" dataDxfId="15"/>
+    <tableColumn id="9" name="DESCRIÇÃO" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A1:F102" totalsRowShown="0" dataDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A1:F102" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:F102"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ID" dataDxfId="116"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="115"/>
-    <tableColumn id="3" name="N° BYTES" dataDxfId="114"/>
-    <tableColumn id="4" name="COMMAND" dataDxfId="113"/>
-    <tableColumn id="5" name="Colunas1" dataDxfId="112"/>
-    <tableColumn id="6" name="DESCRIÇÃO" dataDxfId="111"/>
+    <tableColumn id="1" name="ID" dataDxfId="5"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="4"/>
+    <tableColumn id="3" name="N° BYTES" dataDxfId="3"/>
+    <tableColumn id="4" name="COMMAND" dataDxfId="2"/>
+    <tableColumn id="5" name="Colunas1" dataDxfId="1"/>
+    <tableColumn id="6" name="DESCRIÇÃO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabela10" displayName="Tabela10" ref="A1:K9" totalsRowShown="0" headerRowDxfId="272" dataDxfId="271">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabela10" displayName="Tabela10" ref="A1:K9" totalsRowShown="0" headerRowDxfId="260" dataDxfId="259">
   <autoFilter ref="A1:K9"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="ID" dataDxfId="270"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="269"/>
-    <tableColumn id="3" name="BACK COLOUR" dataDxfId="268"/>
-    <tableColumn id="4" name="SOFT KEY MASK" dataDxfId="267"/>
-    <tableColumn id="5" name="N° OBJETOS" dataDxfId="266"/>
-    <tableColumn id="6" name="N° MACROS" dataDxfId="265"/>
-    <tableColumn id="7" name="OBJ + POS" dataDxfId="264"/>
-    <tableColumn id="8" name="Colunas1" dataDxfId="263"/>
+    <tableColumn id="1" name="ID" dataDxfId="258"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="257"/>
+    <tableColumn id="3" name="BACK COLOUR" dataDxfId="256"/>
+    <tableColumn id="4" name="SOFT KEY MASK" dataDxfId="255"/>
+    <tableColumn id="5" name="N° OBJETOS" dataDxfId="254"/>
+    <tableColumn id="6" name="N° MACROS" dataDxfId="253"/>
+    <tableColumn id="7" name="OBJ + POS" dataDxfId="252"/>
+    <tableColumn id="8" name="Colunas1" dataDxfId="251"/>
     <tableColumn id="9" name="EVENT + MACRO ID"/>
     <tableColumn id="10" name="Colunas2"/>
-    <tableColumn id="11" name="DESCRIÇÃO" dataDxfId="262"/>
+    <tableColumn id="11" name="DESCRIÇÃO" dataDxfId="250"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tabela1025" displayName="Tabela1025" ref="A1:M2" totalsRowShown="0" headerRowDxfId="261" dataDxfId="260">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tabela1025" displayName="Tabela1025" ref="A1:M2" totalsRowShown="0" headerRowDxfId="247" dataDxfId="246">
   <autoFilter ref="A1:M2"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="ID" dataDxfId="259"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="258"/>
-    <tableColumn id="3" name="BACK COLOUR" dataDxfId="257"/>
-    <tableColumn id="4" name="SOFT KEY MASK" dataDxfId="256"/>
-    <tableColumn id="12" name="Priority" dataDxfId="255"/>
-    <tableColumn id="13" name="Acoustic Signal" dataDxfId="254"/>
-    <tableColumn id="5" name="N° OBJETOS" dataDxfId="253"/>
-    <tableColumn id="6" name="N° MACROS" dataDxfId="252"/>
-    <tableColumn id="7" name="OBJ + POS" dataDxfId="251"/>
-    <tableColumn id="8" name="Colunas1" dataDxfId="250"/>
+    <tableColumn id="1" name="ID" dataDxfId="245"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="244"/>
+    <tableColumn id="3" name="BACK COLOUR" dataDxfId="243"/>
+    <tableColumn id="4" name="SOFT KEY MASK" dataDxfId="242"/>
+    <tableColumn id="12" name="Priority" dataDxfId="241"/>
+    <tableColumn id="13" name="Acoustic Signal" dataDxfId="240"/>
+    <tableColumn id="5" name="N° OBJETOS" dataDxfId="239"/>
+    <tableColumn id="6" name="N° MACROS" dataDxfId="238"/>
+    <tableColumn id="7" name="OBJ + POS" dataDxfId="237"/>
+    <tableColumn id="8" name="Colunas1" dataDxfId="236"/>
     <tableColumn id="9" name="EVENT + MACRO ID"/>
     <tableColumn id="10" name="Colunas2"/>
-    <tableColumn id="11" name="DESCRIÇÃO" dataDxfId="249"/>
+    <tableColumn id="11" name="DESCRIÇÃO" dataDxfId="235"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabela15" displayName="Tabela15" ref="A1:K125" totalsRowShown="0" headerRowDxfId="248">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabela15" displayName="Tabela15" ref="A1:K125" totalsRowShown="0" headerRowDxfId="230">
   <autoFilter ref="A1:K125"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID"/>
@@ -15751,7 +15751,7 @@
     <tableColumn id="7" name="FILL ATTRIBUTES"/>
     <tableColumn id="8" name="N° MACRO"/>
     <tableColumn id="9" name="EVENT + MACRO ID"/>
-    <tableColumn id="10" name="Colunas1" dataDxfId="247"/>
+    <tableColumn id="10" name="Colunas1" dataDxfId="229"/>
     <tableColumn id="11" name="DESCRIÇÃO"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -15813,19 +15813,19 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabela11" displayName="Tabela11" ref="A1:J9" totalsRowShown="0" headerRowDxfId="246">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabela11" displayName="Tabela11" ref="A1:J9" totalsRowShown="0" headerRowDxfId="221">
   <autoFilter ref="A1:J9"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="ID" dataDxfId="245"/>
-    <tableColumn id="2" name="TYPE" dataDxfId="244"/>
-    <tableColumn id="3" name="BACK COLOUR" dataDxfId="243"/>
-    <tableColumn id="4" name="N° OBJETOS" dataDxfId="242"/>
-    <tableColumn id="5" name="N° MACROS" dataDxfId="241"/>
-    <tableColumn id="6" name="ID OBJETO" dataDxfId="240"/>
-    <tableColumn id="7" name="Colunas1" dataDxfId="239"/>
+    <tableColumn id="1" name="ID" dataDxfId="220"/>
+    <tableColumn id="2" name="TYPE" dataDxfId="219"/>
+    <tableColumn id="3" name="BACK COLOUR" dataDxfId="218"/>
+    <tableColumn id="4" name="N° OBJETOS" dataDxfId="217"/>
+    <tableColumn id="5" name="N° MACROS" dataDxfId="216"/>
+    <tableColumn id="6" name="ID OBJETO" dataDxfId="215"/>
+    <tableColumn id="7" name="Colunas1" dataDxfId="214"/>
     <tableColumn id="8" name="EVENT + MACRO ID"/>
-    <tableColumn id="9" name="Colunas2" dataDxfId="238"/>
-    <tableColumn id="10" name="DESCRIÇÃO" dataDxfId="237"/>
+    <tableColumn id="9" name="Colunas2" dataDxfId="213"/>
+    <tableColumn id="10" name="DESCRIÇÃO" dataDxfId="212"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17239,62 +17239,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H16">
-    <cfRule type="expression" dxfId="85" priority="12">
+    <cfRule type="expression" dxfId="211" priority="12">
       <formula>IF(HEX2DEC(RIGHT(E2,2))&gt;0,(IF((HEX2DEC(RIGHT(E2,2))*36-2)=LEN(G2),1,0)),(IF((HEX2DEC(RIGHT(E2,2))*36)=LEN(G2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J16">
-    <cfRule type="expression" dxfId="84" priority="11">
+    <cfRule type="expression" dxfId="210" priority="11">
       <formula>IF(HEX2DEC(RIGHT(F2,2))&gt;0,(IF((HEX2DEC(RIGHT(F2,2))*12-2)=LEN(I2),1,0)),(IF((HEX2DEC(RIGHT(F2,2))*12)=LEN(I2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="expression" dxfId="83" priority="10">
+    <cfRule type="expression" dxfId="209" priority="10">
       <formula>IF(HEX2DEC(RIGHT(E13,2))&gt;0,(IF((HEX2DEC(RIGHT(E13,2))*36-2)=LEN(G13),1,0)),(IF((HEX2DEC(RIGHT(E13,2))*36)=LEN(G13),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="expression" dxfId="82" priority="9">
+    <cfRule type="expression" dxfId="208" priority="9">
       <formula>IF(HEX2DEC(RIGHT(F13,2))&gt;0,(IF((HEX2DEC(RIGHT(F13,2))*12-2)=LEN(I13),1,0)),(IF((HEX2DEC(RIGHT(F13,2))*12)=LEN(I13),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="expression" dxfId="81" priority="8">
+    <cfRule type="expression" dxfId="207" priority="8">
       <formula>IF(HEX2DEC(RIGHT(E14,2))&gt;0,(IF((HEX2DEC(RIGHT(E14,2))*36-2)=LEN(G14),1,0)),(IF((HEX2DEC(RIGHT(E14,2))*36)=LEN(G14),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="expression" dxfId="80" priority="7">
+    <cfRule type="expression" dxfId="206" priority="7">
       <formula>IF(HEX2DEC(RIGHT(F14,2))&gt;0,(IF((HEX2DEC(RIGHT(F14,2))*12-2)=LEN(I14),1,0)),(IF((HEX2DEC(RIGHT(F14,2))*12)=LEN(I14),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="expression" dxfId="79" priority="6">
+    <cfRule type="expression" dxfId="205" priority="6">
       <formula>IF(HEX2DEC(RIGHT(E15,2))&gt;0,(IF((HEX2DEC(RIGHT(E15,2))*36-2)=LEN(G15),1,0)),(IF((HEX2DEC(RIGHT(E15,2))*36)=LEN(G15),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="expression" dxfId="78" priority="5">
+    <cfRule type="expression" dxfId="204" priority="5">
       <formula>IF(HEX2DEC(RIGHT(F15,2))&gt;0,(IF((HEX2DEC(RIGHT(F15,2))*12-2)=LEN(I15),1,0)),(IF((HEX2DEC(RIGHT(F15,2))*12)=LEN(I15),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="expression" dxfId="77" priority="4">
+    <cfRule type="expression" dxfId="203" priority="4">
       <formula>IF(HEX2DEC(RIGHT(E15,2))&gt;0,(IF((HEX2DEC(RIGHT(E15,2))*36-2)=LEN(G15),1,0)),(IF((HEX2DEC(RIGHT(E15,2))*36)=LEN(G15),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15">
-    <cfRule type="expression" dxfId="76" priority="3">
+    <cfRule type="expression" dxfId="202" priority="3">
       <formula>IF(HEX2DEC(RIGHT(F15,2))&gt;0,(IF((HEX2DEC(RIGHT(F15,2))*12-2)=LEN(I15),1,0)),(IF((HEX2DEC(RIGHT(F15,2))*12)=LEN(I15),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="expression" dxfId="75" priority="2">
+    <cfRule type="expression" dxfId="201" priority="2">
       <formula>IF(HEX2DEC(RIGHT(E16,2))&gt;0,(IF((HEX2DEC(RIGHT(E16,2))*36-2)=LEN(G16),1,0)),(IF((HEX2DEC(RIGHT(E16,2))*36)=LEN(G16),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="expression" dxfId="74" priority="1">
+    <cfRule type="expression" dxfId="200" priority="1">
       <formula>IF(HEX2DEC(RIGHT(F16,2))&gt;0,(IF((HEX2DEC(RIGHT(F16,2))*12-2)=LEN(I16),1,0)),(IF((HEX2DEC(RIGHT(F16,2))*12)=LEN(I16),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21647,42 +21647,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I135">
-    <cfRule type="expression" dxfId="73" priority="8">
+    <cfRule type="expression" dxfId="186" priority="8">
       <formula>IF(HEX2DEC(RIGHT(F2,2))&gt;0,(IF((HEX2DEC(RIGHT(F2,2))*36-2)=LEN(H2),1,0)),(IF((HEX2DEC(RIGHT(F2,2))*36)=LEN(H2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K135">
-    <cfRule type="expression" dxfId="72" priority="7">
+    <cfRule type="expression" dxfId="185" priority="7">
       <formula>IF(HEX2DEC(RIGHT(G2,2))&gt;0,(IF((HEX2DEC(RIGHT(G2,2))*12-2)=LEN(J2),1,0)),(IF((HEX2DEC(RIGHT(G2,2))*12)=LEN(J2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I134">
-    <cfRule type="expression" dxfId="71" priority="6">
+    <cfRule type="expression" dxfId="184" priority="6">
       <formula>IF(HEX2DEC(RIGHT(F134,2))&gt;0,(IF((HEX2DEC(RIGHT(F134,2))*36-2)=LEN(H134),1,0)),(IF((HEX2DEC(RIGHT(F134,2))*36)=LEN(H134),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K134">
-    <cfRule type="expression" dxfId="70" priority="5">
+    <cfRule type="expression" dxfId="183" priority="5">
       <formula>IF(HEX2DEC(RIGHT(G134,2))&gt;0,(IF((HEX2DEC(RIGHT(G134,2))*12-2)=LEN(J134),1,0)),(IF((HEX2DEC(RIGHT(G134,2))*12)=LEN(J134),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I135">
-    <cfRule type="expression" dxfId="69" priority="4">
+    <cfRule type="expression" dxfId="182" priority="4">
       <formula>IF(HEX2DEC(RIGHT(F135,2))&gt;0,(IF((HEX2DEC(RIGHT(F135,2))*36-2)=LEN(H135),1,0)),(IF((HEX2DEC(RIGHT(F135,2))*36)=LEN(H135),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K135">
-    <cfRule type="expression" dxfId="68" priority="3">
+    <cfRule type="expression" dxfId="181" priority="3">
       <formula>IF(HEX2DEC(RIGHT(G135,2))&gt;0,(IF((HEX2DEC(RIGHT(G135,2))*12-2)=LEN(J135),1,0)),(IF((HEX2DEC(RIGHT(G135,2))*12)=LEN(J135),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I135">
-    <cfRule type="expression" dxfId="67" priority="2">
+    <cfRule type="expression" dxfId="180" priority="2">
       <formula>IF(HEX2DEC(RIGHT(F135,2))&gt;0,(IF((HEX2DEC(RIGHT(F135,2))*36-2)=LEN(H135),1,0)),(IF((HEX2DEC(RIGHT(F135,2))*36)=LEN(H135),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K135">
-    <cfRule type="expression" dxfId="66" priority="1">
+    <cfRule type="expression" dxfId="179" priority="1">
       <formula>IF(HEX2DEC(RIGHT(G135,2))&gt;0,(IF((HEX2DEC(RIGHT(G135,2))*12-2)=LEN(J135),1,0)),(IF((HEX2DEC(RIGHT(G135,2))*12)=LEN(J135),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21700,7 +21700,7 @@
   <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
@@ -24140,192 +24140,192 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L58">
-    <cfRule type="expression" dxfId="65" priority="40">
+    <cfRule type="expression" dxfId="165" priority="40">
       <formula>IF(HEX2DEC(RIGHT(I2,2))&gt;0,(IF((HEX2DEC(RIGHT(I2,2))*36-2)=LEN(K2),1,0)),(IF((HEX2DEC(RIGHT(I2,2))*36)=LEN(K2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N58">
-    <cfRule type="expression" dxfId="64" priority="39">
+    <cfRule type="expression" dxfId="164" priority="39">
       <formula>IF(HEX2DEC(RIGHT(J2,2))&gt;0,(IF((HEX2DEC(RIGHT(J2,2))*12-2)=LEN(M2),1,0)),(IF((HEX2DEC(RIGHT(J2,2))*12)=LEN(M2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L54">
-    <cfRule type="expression" dxfId="63" priority="36">
+    <cfRule type="expression" dxfId="163" priority="36">
       <formula>IF(HEX2DEC(RIGHT(I54,2))&gt;0,(IF((HEX2DEC(RIGHT(I54,2))*36-2)=LEN(K54),1,0)),(IF((HEX2DEC(RIGHT(I54,2))*36)=LEN(K54),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N54">
-    <cfRule type="expression" dxfId="62" priority="35">
+    <cfRule type="expression" dxfId="162" priority="35">
       <formula>IF(HEX2DEC(RIGHT(J54,2))&gt;0,(IF((HEX2DEC(RIGHT(J54,2))*12-2)=LEN(M54),1,0)),(IF((HEX2DEC(RIGHT(J54,2))*12)=LEN(M54),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L54">
-    <cfRule type="expression" dxfId="61" priority="34">
+    <cfRule type="expression" dxfId="161" priority="34">
       <formula>IF(HEX2DEC(RIGHT(I54,2))&gt;0,(IF((HEX2DEC(RIGHT(I54,2))*36-2)=LEN(K54),1,0)),(IF((HEX2DEC(RIGHT(I54,2))*36)=LEN(K54),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N54">
-    <cfRule type="expression" dxfId="60" priority="33">
+    <cfRule type="expression" dxfId="160" priority="33">
       <formula>IF(HEX2DEC(RIGHT(J54,2))&gt;0,(IF((HEX2DEC(RIGHT(J54,2))*12-2)=LEN(M54),1,0)),(IF((HEX2DEC(RIGHT(J54,2))*12)=LEN(M54),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55">
-    <cfRule type="expression" dxfId="59" priority="32">
+    <cfRule type="expression" dxfId="159" priority="32">
       <formula>IF(HEX2DEC(RIGHT(I55,2))&gt;0,(IF((HEX2DEC(RIGHT(I55,2))*36-2)=LEN(K55),1,0)),(IF((HEX2DEC(RIGHT(I55,2))*36)=LEN(K55),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55">
-    <cfRule type="expression" dxfId="58" priority="31">
+    <cfRule type="expression" dxfId="158" priority="31">
       <formula>IF(HEX2DEC(RIGHT(J55,2))&gt;0,(IF((HEX2DEC(RIGHT(J55,2))*12-2)=LEN(M55),1,0)),(IF((HEX2DEC(RIGHT(J55,2))*12)=LEN(M55),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55">
-    <cfRule type="expression" dxfId="57" priority="30">
+    <cfRule type="expression" dxfId="157" priority="30">
       <formula>IF(HEX2DEC(RIGHT(I55,2))&gt;0,(IF((HEX2DEC(RIGHT(I55,2))*36-2)=LEN(K55),1,0)),(IF((HEX2DEC(RIGHT(I55,2))*36)=LEN(K55),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55">
-    <cfRule type="expression" dxfId="56" priority="29">
+    <cfRule type="expression" dxfId="156" priority="29">
       <formula>IF(HEX2DEC(RIGHT(J55,2))&gt;0,(IF((HEX2DEC(RIGHT(J55,2))*12-2)=LEN(M55),1,0)),(IF((HEX2DEC(RIGHT(J55,2))*12)=LEN(M55),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55">
-    <cfRule type="expression" dxfId="55" priority="28">
+    <cfRule type="expression" dxfId="155" priority="28">
       <formula>IF(HEX2DEC(RIGHT(I55,2))&gt;0,(IF((HEX2DEC(RIGHT(I55,2))*36-2)=LEN(K55),1,0)),(IF((HEX2DEC(RIGHT(I55,2))*36)=LEN(K55),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55">
-    <cfRule type="expression" dxfId="54" priority="27">
+    <cfRule type="expression" dxfId="154" priority="27">
       <formula>IF(HEX2DEC(RIGHT(J55,2))&gt;0,(IF((HEX2DEC(RIGHT(J55,2))*12-2)=LEN(M55),1,0)),(IF((HEX2DEC(RIGHT(J55,2))*12)=LEN(M55),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N58">
-    <cfRule type="expression" dxfId="53" priority="1">
+    <cfRule type="expression" dxfId="153" priority="1">
       <formula>IF(HEX2DEC(RIGHT(J58,2))&gt;0,(IF((HEX2DEC(RIGHT(J58,2))*12-2)=LEN(M58),1,0)),(IF((HEX2DEC(RIGHT(J58,2))*12)=LEN(M58),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="expression" dxfId="52" priority="26">
+    <cfRule type="expression" dxfId="152" priority="26">
       <formula>IF(HEX2DEC(RIGHT(I56,2))&gt;0,(IF((HEX2DEC(RIGHT(I56,2))*36-2)=LEN(K56),1,0)),(IF((HEX2DEC(RIGHT(I56,2))*36)=LEN(K56),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56">
-    <cfRule type="expression" dxfId="51" priority="25">
+    <cfRule type="expression" dxfId="151" priority="25">
       <formula>IF(HEX2DEC(RIGHT(J56,2))&gt;0,(IF((HEX2DEC(RIGHT(J56,2))*12-2)=LEN(M56),1,0)),(IF((HEX2DEC(RIGHT(J56,2))*12)=LEN(M56),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="expression" dxfId="50" priority="24">
+    <cfRule type="expression" dxfId="150" priority="24">
       <formula>IF(HEX2DEC(RIGHT(I56,2))&gt;0,(IF((HEX2DEC(RIGHT(I56,2))*36-2)=LEN(K56),1,0)),(IF((HEX2DEC(RIGHT(I56,2))*36)=LEN(K56),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56">
-    <cfRule type="expression" dxfId="49" priority="23">
+    <cfRule type="expression" dxfId="149" priority="23">
       <formula>IF(HEX2DEC(RIGHT(J56,2))&gt;0,(IF((HEX2DEC(RIGHT(J56,2))*12-2)=LEN(M56),1,0)),(IF((HEX2DEC(RIGHT(J56,2))*12)=LEN(M56),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="expression" dxfId="48" priority="22">
+    <cfRule type="expression" dxfId="148" priority="22">
       <formula>IF(HEX2DEC(RIGHT(I56,2))&gt;0,(IF((HEX2DEC(RIGHT(I56,2))*36-2)=LEN(K56),1,0)),(IF((HEX2DEC(RIGHT(I56,2))*36)=LEN(K56),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56">
-    <cfRule type="expression" dxfId="47" priority="21">
+    <cfRule type="expression" dxfId="147" priority="21">
       <formula>IF(HEX2DEC(RIGHT(J56,2))&gt;0,(IF((HEX2DEC(RIGHT(J56,2))*12-2)=LEN(M56),1,0)),(IF((HEX2DEC(RIGHT(J56,2))*12)=LEN(M56),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="expression" dxfId="46" priority="20">
+    <cfRule type="expression" dxfId="146" priority="20">
       <formula>IF(HEX2DEC(RIGHT(I56,2))&gt;0,(IF((HEX2DEC(RIGHT(I56,2))*36-2)=LEN(K56),1,0)),(IF((HEX2DEC(RIGHT(I56,2))*36)=LEN(K56),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56">
-    <cfRule type="expression" dxfId="45" priority="19">
+    <cfRule type="expression" dxfId="145" priority="19">
       <formula>IF(HEX2DEC(RIGHT(J56,2))&gt;0,(IF((HEX2DEC(RIGHT(J56,2))*12-2)=LEN(M56),1,0)),(IF((HEX2DEC(RIGHT(J56,2))*12)=LEN(M56),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57">
-    <cfRule type="expression" dxfId="44" priority="18">
+    <cfRule type="expression" dxfId="144" priority="18">
       <formula>IF(HEX2DEC(RIGHT(I57,2))&gt;0,(IF((HEX2DEC(RIGHT(I57,2))*36-2)=LEN(K57),1,0)),(IF((HEX2DEC(RIGHT(I57,2))*36)=LEN(K57),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57">
-    <cfRule type="expression" dxfId="43" priority="17">
+    <cfRule type="expression" dxfId="143" priority="17">
       <formula>IF(HEX2DEC(RIGHT(J57,2))&gt;0,(IF((HEX2DEC(RIGHT(J57,2))*12-2)=LEN(M57),1,0)),(IF((HEX2DEC(RIGHT(J57,2))*12)=LEN(M57),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57">
-    <cfRule type="expression" dxfId="42" priority="16">
+    <cfRule type="expression" dxfId="142" priority="16">
       <formula>IF(HEX2DEC(RIGHT(I57,2))&gt;0,(IF((HEX2DEC(RIGHT(I57,2))*36-2)=LEN(K57),1,0)),(IF((HEX2DEC(RIGHT(I57,2))*36)=LEN(K57),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57">
-    <cfRule type="expression" dxfId="41" priority="15">
+    <cfRule type="expression" dxfId="141" priority="15">
       <formula>IF(HEX2DEC(RIGHT(J57,2))&gt;0,(IF((HEX2DEC(RIGHT(J57,2))*12-2)=LEN(M57),1,0)),(IF((HEX2DEC(RIGHT(J57,2))*12)=LEN(M57),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57">
-    <cfRule type="expression" dxfId="40" priority="14">
+    <cfRule type="expression" dxfId="140" priority="14">
       <formula>IF(HEX2DEC(RIGHT(I57,2))&gt;0,(IF((HEX2DEC(RIGHT(I57,2))*36-2)=LEN(K57),1,0)),(IF((HEX2DEC(RIGHT(I57,2))*36)=LEN(K57),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57">
-    <cfRule type="expression" dxfId="39" priority="13">
+    <cfRule type="expression" dxfId="139" priority="13">
       <formula>IF(HEX2DEC(RIGHT(J57,2))&gt;0,(IF((HEX2DEC(RIGHT(J57,2))*12-2)=LEN(M57),1,0)),(IF((HEX2DEC(RIGHT(J57,2))*12)=LEN(M57),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L57">
-    <cfRule type="expression" dxfId="38" priority="12">
+    <cfRule type="expression" dxfId="138" priority="12">
       <formula>IF(HEX2DEC(RIGHT(I57,2))&gt;0,(IF((HEX2DEC(RIGHT(I57,2))*36-2)=LEN(K57),1,0)),(IF((HEX2DEC(RIGHT(I57,2))*36)=LEN(K57),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N57">
-    <cfRule type="expression" dxfId="37" priority="11">
+    <cfRule type="expression" dxfId="137" priority="11">
       <formula>IF(HEX2DEC(RIGHT(J57,2))&gt;0,(IF((HEX2DEC(RIGHT(J57,2))*12-2)=LEN(M57),1,0)),(IF((HEX2DEC(RIGHT(J57,2))*12)=LEN(M57),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58">
-    <cfRule type="expression" dxfId="36" priority="10">
+    <cfRule type="expression" dxfId="136" priority="10">
       <formula>IF(HEX2DEC(RIGHT(I58,2))&gt;0,(IF((HEX2DEC(RIGHT(I58,2))*36-2)=LEN(K58),1,0)),(IF((HEX2DEC(RIGHT(I58,2))*36)=LEN(K58),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N58">
-    <cfRule type="expression" dxfId="35" priority="9">
+    <cfRule type="expression" dxfId="135" priority="9">
       <formula>IF(HEX2DEC(RIGHT(J58,2))&gt;0,(IF((HEX2DEC(RIGHT(J58,2))*12-2)=LEN(M58),1,0)),(IF((HEX2DEC(RIGHT(J58,2))*12)=LEN(M58),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58">
-    <cfRule type="expression" dxfId="34" priority="8">
+    <cfRule type="expression" dxfId="134" priority="8">
       <formula>IF(HEX2DEC(RIGHT(I58,2))&gt;0,(IF((HEX2DEC(RIGHT(I58,2))*36-2)=LEN(K58),1,0)),(IF((HEX2DEC(RIGHT(I58,2))*36)=LEN(K58),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N58">
-    <cfRule type="expression" dxfId="33" priority="7">
+    <cfRule type="expression" dxfId="133" priority="7">
       <formula>IF(HEX2DEC(RIGHT(J58,2))&gt;0,(IF((HEX2DEC(RIGHT(J58,2))*12-2)=LEN(M58),1,0)),(IF((HEX2DEC(RIGHT(J58,2))*12)=LEN(M58),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58">
-    <cfRule type="expression" dxfId="32" priority="6">
+    <cfRule type="expression" dxfId="132" priority="6">
       <formula>IF(HEX2DEC(RIGHT(I58,2))&gt;0,(IF((HEX2DEC(RIGHT(I58,2))*36-2)=LEN(K58),1,0)),(IF((HEX2DEC(RIGHT(I58,2))*36)=LEN(K58),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N58">
-    <cfRule type="expression" dxfId="31" priority="5">
+    <cfRule type="expression" dxfId="131" priority="5">
       <formula>IF(HEX2DEC(RIGHT(J58,2))&gt;0,(IF((HEX2DEC(RIGHT(J58,2))*12-2)=LEN(M58),1,0)),(IF((HEX2DEC(RIGHT(J58,2))*12)=LEN(M58),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58">
-    <cfRule type="expression" dxfId="30" priority="4">
+    <cfRule type="expression" dxfId="130" priority="4">
       <formula>IF(HEX2DEC(RIGHT(I58,2))&gt;0,(IF((HEX2DEC(RIGHT(I58,2))*36-2)=LEN(K58),1,0)),(IF((HEX2DEC(RIGHT(I58,2))*36)=LEN(K58),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N58">
-    <cfRule type="expression" dxfId="29" priority="3">
+    <cfRule type="expression" dxfId="129" priority="3">
       <formula>IF(HEX2DEC(RIGHT(J58,2))&gt;0,(IF((HEX2DEC(RIGHT(J58,2))*12-2)=LEN(M58),1,0)),(IF((HEX2DEC(RIGHT(J58,2))*12)=LEN(M58),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L58">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="128" priority="2">
       <formula>IF(HEX2DEC(RIGHT(I58,2))&gt;0,(IF((HEX2DEC(RIGHT(I58,2))*36-2)=LEN(K58),1,0)),(IF((HEX2DEC(RIGHT(I58,2))*36)=LEN(K58),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24467,7 +24467,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K2:K3">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="111" priority="1">
       <formula>IF(HEX2DEC(RIGHT(I2,2))&gt;0,(IF((HEX2DEC(RIGHT(I2,2))*12-2)=LEN(J2),1,0)),(IF((HEX2DEC(RIGHT(I2,2))*12)=LEN(J2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24483,8 +24483,8 @@
   <sheetPr codeName="Plan8"/>
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="A7:N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="A5:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24717,7 +24717,7 @@
         <v>45</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>83</v>
@@ -24778,7 +24778,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K2:K7 M2:M7">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="109" priority="2">
       <formula>IF(HEX2DEC(RIGHT(G2,2))&gt;0,(IF((HEX2DEC(RIGHT(G2,2))*12-2)=LEN(J2),1,0)),(IF((HEX2DEC(RIGHT(G2,2))*12)=LEN(J2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24794,9 +24794,9 @@
   <sheetPr codeName="Plan9"/>
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="R11" sqref="A11:R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25491,7 +25491,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="T2:T11">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="93" priority="1">
       <formula>IF(HEX2DEC(RIGHT(R2,2))&gt;0,(IF((HEX2DEC(RIGHT(R2,2))*12-2)=LEN(S2),1,0)),(IF((HEX2DEC(RIGHT(R2,2))*12)=LEN(S2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49223,7 +49223,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q2:Q145">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="72" priority="1">
       <formula>IF(HEX2DEC(RIGHT(O2,2))&gt;0,(IF((HEX2DEC(RIGHT(O2,2))*12-2)=LEN(P2),1,0)),(IF((HEX2DEC(RIGHT(O2,2))*12)=LEN(P2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -49240,7 +49240,7 @@
   <dimension ref="A1:E483"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D483" sqref="D483"/>
     </sheetView>
   </sheetViews>
@@ -68559,68 +68559,68 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L296">
-    <cfRule type="expression" dxfId="23" priority="16">
+    <cfRule type="expression" dxfId="69" priority="16">
       <formula>IF(HEX2DEC(MID(J2,3,2))&gt;0,(IF(((HEX2DEC(MID(J2,3,2))*6)-2)=LEN(K2),1,0)),(IF((HEX2DEC(MID(J2,3,2))*6)=LEN(K2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L293">
-    <cfRule type="expression" dxfId="22" priority="13">
+    <cfRule type="expression" dxfId="68" priority="13">
       <formula>IF(HEX2DEC(MID(J293,3,2))&gt;0,(IF(((HEX2DEC(MID(J293,3,2))*6)-2)=LEN(K293),1,0)),(IF((HEX2DEC(MID(J293,3,2))*6)=LEN(K293),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N293">
-    <cfRule type="duplicateValues" dxfId="21" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L294">
-    <cfRule type="expression" dxfId="20" priority="11">
+    <cfRule type="expression" dxfId="66" priority="11">
       <formula>IF(HEX2DEC(MID(J294,3,2))&gt;0,(IF(((HEX2DEC(MID(J294,3,2))*6)-2)=LEN(K294),1,0)),(IF((HEX2DEC(MID(J294,3,2))*6)=LEN(K294),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N294">
-    <cfRule type="duplicateValues" dxfId="19" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L295">
-    <cfRule type="expression" dxfId="18" priority="9">
+    <cfRule type="expression" dxfId="64" priority="9">
       <formula>IF(HEX2DEC(MID(J295,3,2))&gt;0,(IF(((HEX2DEC(MID(J295,3,2))*6)-2)=LEN(K295),1,0)),(IF((HEX2DEC(MID(J295,3,2))*6)=LEN(K295),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N295">
-    <cfRule type="duplicateValues" dxfId="17" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L295">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="62" priority="7">
       <formula>IF(HEX2DEC(MID(J295,3,2))&gt;0,(IF(((HEX2DEC(MID(J295,3,2))*6)-2)=LEN(K295),1,0)),(IF((HEX2DEC(MID(J295,3,2))*6)=LEN(K295),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N295">
-    <cfRule type="duplicateValues" dxfId="15" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N296">
-    <cfRule type="duplicateValues" dxfId="14" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L296">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="59" priority="5">
       <formula>IF(HEX2DEC(MID(J296,3,2))&gt;0,(IF(((HEX2DEC(MID(J296,3,2))*6)-2)=LEN(K296),1,0)),(IF((HEX2DEC(MID(J296,3,2))*6)=LEN(K296),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L296">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="58" priority="3">
       <formula>IF(HEX2DEC(MID(J296,3,2))&gt;0,(IF(((HEX2DEC(MID(J296,3,2))*6)-2)=LEN(K296),1,0)),(IF((HEX2DEC(MID(J296,3,2))*6)=LEN(K296),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N296">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L296">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="56" priority="1">
       <formula>IF(HEX2DEC(MID(J296,3,2))&gt;0,(IF(((HEX2DEC(MID(J296,3,2))*6)-2)=LEN(K296),1,0)),(IF((HEX2DEC(MID(J296,3,2))*6)=LEN(K296),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N296">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N296">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -68739,12 +68739,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2">
-    <cfRule type="expression" dxfId="110" priority="2">
+    <cfRule type="expression" dxfId="288" priority="2">
       <formula>IF(HEX2DEC(RIGHT(F2,2))&gt;0,(IF((HEX2DEC(RIGHT(F2,2))*36-2)=LEN(I2),1,0)),(IF((HEX2DEC(RIGHT(F2,2))*36)=LEN(I2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="109" priority="1">
+    <cfRule type="expression" dxfId="287" priority="1">
       <formula>IF(HEX2DEC(RIGHT(G2,2))&gt;0,(IF((HEX2DEC(RIGHT(G2,2))*12-2)=LEN(K2),1,0)),(IF((HEX2DEC(RIGHT(G2,2))*12)=LEN(K2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -69455,7 +69455,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I12">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>IF(HEX2DEC(RIGHT(G2,2))&gt;0,(IF((HEX2DEC(RIGHT(G2,2))*12-2)=LEN(H2),1,0)),(IF((HEX2DEC(RIGHT(G2,2))*12)=LEN(H2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -71292,37 +71292,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E102">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="13" priority="8">
       <formula>IF(HEX2DEC(MID(C2,3,2))&gt;0,(IF(((HEX2DEC(MID(C2,3,2))*6)-2)=LEN(D2),1,0)),(IF((HEX2DEC(MID(C2,3,2))*6)=LEN(D2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E100">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="12" priority="7">
       <formula>IF(HEX2DEC(MID(C100,3,2))&gt;0,(IF(((HEX2DEC(MID(C100,3,2))*6)-2)=LEN(D100),1,0)),(IF((HEX2DEC(MID(C100,3,2))*6)=LEN(D100),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E101">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>IF(HEX2DEC(MID(C101,3,2))&gt;0,(IF(((HEX2DEC(MID(C101,3,2))*6)-2)=LEN(D101),1,0)),(IF((HEX2DEC(MID(C101,3,2))*6)=LEN(D101),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E101">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>IF(HEX2DEC(MID(C101,3,2))&gt;0,(IF(((HEX2DEC(MID(C101,3,2))*6)-2)=LEN(D101),1,0)),(IF((HEX2DEC(MID(C101,3,2))*6)=LEN(D101),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>IF(HEX2DEC(MID(C102,3,2))&gt;0,(IF(((HEX2DEC(MID(C102,3,2))*6)-2)=LEN(D102),1,0)),(IF((HEX2DEC(MID(C102,3,2))*6)=LEN(D102),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>IF(HEX2DEC(MID(C102,3,2))&gt;0,(IF(((HEX2DEC(MID(C102,3,2))*6)-2)=LEN(D102),1,0)),(IF((HEX2DEC(MID(C102,3,2))*6)=LEN(D102),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>IF(HEX2DEC(MID(C102,3,2))&gt;0,(IF(((HEX2DEC(MID(C102,3,2))*6)-2)=LEN(D102),1,0)),(IF((HEX2DEC(MID(C102,3,2))*6)=LEN(D102),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -71611,52 +71611,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H9">
-    <cfRule type="expression" dxfId="108" priority="10">
+    <cfRule type="expression" dxfId="270" priority="10">
       <formula>IF(HEX2DEC(RIGHT(E2,2))&gt;0,(IF((HEX2DEC(RIGHT(E2,2))*36-2)=LEN(G2),1,0)),(IF((HEX2DEC(RIGHT(E2,2))*36)=LEN(G2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J9">
-    <cfRule type="expression" dxfId="107" priority="9">
+    <cfRule type="expression" dxfId="269" priority="9">
       <formula>IF(HEX2DEC(RIGHT(F2,2))&gt;0,(IF((HEX2DEC(RIGHT(F2,2))*12-2)=LEN(I2),1,0)),(IF((HEX2DEC(RIGHT(F2,2))*12)=LEN(I2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="106" priority="8">
+    <cfRule type="expression" dxfId="268" priority="8">
       <formula>IF(HEX2DEC(RIGHT(E5,2))&gt;0,(IF((HEX2DEC(RIGHT(E5,2))*36-2)=LEN(G5),1,0)),(IF((HEX2DEC(RIGHT(E5,2))*36)=LEN(G5),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
-    <cfRule type="expression" dxfId="105" priority="7">
+    <cfRule type="expression" dxfId="267" priority="7">
       <formula>IF(HEX2DEC(RIGHT(F5,2))&gt;0,(IF((HEX2DEC(RIGHT(F5,2))*12-2)=LEN(I5),1,0)),(IF((HEX2DEC(RIGHT(F5,2))*12)=LEN(I5),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="104" priority="6">
+    <cfRule type="expression" dxfId="266" priority="6">
       <formula>IF(HEX2DEC(RIGHT(E8,2))&gt;0,(IF((HEX2DEC(RIGHT(E8,2))*36-2)=LEN(G8),1,0)),(IF((HEX2DEC(RIGHT(E8,2))*36)=LEN(G8),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="103" priority="5">
+    <cfRule type="expression" dxfId="265" priority="5">
       <formula>IF(HEX2DEC(RIGHT(F8,2))&gt;0,(IF((HEX2DEC(RIGHT(F8,2))*12-2)=LEN(I8),1,0)),(IF((HEX2DEC(RIGHT(F8,2))*12)=LEN(I8),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="102" priority="4">
+    <cfRule type="expression" dxfId="264" priority="4">
       <formula>IF(HEX2DEC(RIGHT(E9,2))&gt;0,(IF((HEX2DEC(RIGHT(E9,2))*36-2)=LEN(G9),1,0)),(IF((HEX2DEC(RIGHT(E9,2))*36)=LEN(G9),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="expression" dxfId="101" priority="3">
+    <cfRule type="expression" dxfId="263" priority="3">
       <formula>IF(HEX2DEC(RIGHT(F9,2))&gt;0,(IF((HEX2DEC(RIGHT(F9,2))*12-2)=LEN(I9),1,0)),(IF((HEX2DEC(RIGHT(F9,2))*12)=LEN(I9),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="100" priority="2">
+    <cfRule type="expression" dxfId="262" priority="2">
       <formula>IF(HEX2DEC(RIGHT(E9,2))&gt;0,(IF((HEX2DEC(RIGHT(E9,2))*36-2)=LEN(G9),1,0)),(IF((HEX2DEC(RIGHT(E9,2))*36)=LEN(G9),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="expression" dxfId="99" priority="1">
+    <cfRule type="expression" dxfId="261" priority="1">
       <formula>IF(HEX2DEC(RIGHT(F9,2))&gt;0,(IF((HEX2DEC(RIGHT(F9,2))*12-2)=LEN(I9),1,0)),(IF((HEX2DEC(RIGHT(F9,2))*12)=LEN(I9),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -71769,12 +71769,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2">
-    <cfRule type="expression" dxfId="98" priority="4">
+    <cfRule type="expression" dxfId="249" priority="4">
       <formula>IF(HEX2DEC(RIGHT(G2,2))&gt;0,(IF((HEX2DEC(RIGHT(G2,2))*36-2)=LEN(I2),1,0)),(IF((HEX2DEC(RIGHT(G2,2))*36)=LEN(I2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="97" priority="3">
+    <cfRule type="expression" dxfId="248" priority="3">
       <formula>IF(HEX2DEC(RIGHT(H2,2))&gt;0,(IF((HEX2DEC(RIGHT(H2,2))*12-2)=LEN(K2),1,0)),(IF((HEX2DEC(RIGHT(H2,2))*12)=LEN(K2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -75564,22 +75564,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J125">
-    <cfRule type="expression" dxfId="96" priority="4">
+    <cfRule type="expression" dxfId="234" priority="4">
       <formula>IF(HEX2DEC(RIGHT(H2,2))&gt;0,(IF((HEX2DEC(RIGHT(H2,2))*12-2)=LEN(I2),1,0)),(IF((HEX2DEC(RIGHT(H2,2))*12)=LEN(I2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J123:J124">
-    <cfRule type="expression" dxfId="95" priority="3">
+    <cfRule type="expression" dxfId="233" priority="3">
       <formula>IF(HEX2DEC(RIGHT(H123,2))&gt;0,(IF((HEX2DEC(RIGHT(H123,2))*12-2)=LEN(I123),1,0)),(IF((HEX2DEC(RIGHT(H123,2))*12)=LEN(I123),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J125">
-    <cfRule type="expression" dxfId="94" priority="2">
+    <cfRule type="expression" dxfId="232" priority="2">
       <formula>IF(HEX2DEC(RIGHT(H125,2))&gt;0,(IF((HEX2DEC(RIGHT(H125,2))*12-2)=LEN(I125),1,0)),(IF((HEX2DEC(RIGHT(H125,2))*12)=LEN(I125),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J125">
-    <cfRule type="expression" dxfId="93" priority="1">
+    <cfRule type="expression" dxfId="231" priority="1">
       <formula>IF(HEX2DEC(RIGHT(H125,2))&gt;0,(IF((HEX2DEC(RIGHT(H125,2))*12-2)=LEN(I125),1,0)),(IF((HEX2DEC(RIGHT(H125,2))*12)=LEN(I125),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -77583,12 +77583,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H7 H9">
-    <cfRule type="expression" dxfId="92" priority="3">
+    <cfRule type="expression" dxfId="228" priority="3">
       <formula>IF(HEX2DEC(RIGHT(F2,2))&gt;0,(IF((HEX2DEC(RIGHT(F2,2))*12-2)=LEN(G2),1,0)),(IF((HEX2DEC(RIGHT(F2,2))*12)=LEN(G2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="91" priority="1">
+    <cfRule type="expression" dxfId="227" priority="1">
       <formula>IF(HEX2DEC(RIGHT(F8,2))&gt;0,(IF((HEX2DEC(RIGHT(F8,2))*12-2)=LEN(G8),1,0)),(IF((HEX2DEC(RIGHT(F8,2))*12)=LEN(G8),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -77940,7 +77940,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I12">
-    <cfRule type="expression" dxfId="90" priority="1">
+    <cfRule type="expression" dxfId="226" priority="1">
       <formula>IF(HEX2DEC(RIGHT(G2,2))&gt;0,(IF((HEX2DEC(RIGHT(G2,2))*12-2)=LEN(H2),1,0)),(IF((HEX2DEC(RIGHT(G2,2))*12)=LEN(H2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -78208,22 +78208,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G9">
-    <cfRule type="expression" dxfId="89" priority="6">
+    <cfRule type="expression" dxfId="225" priority="6">
       <formula>IF(HEX2DEC(RIGHT(D2,2))&gt;0,(IF((HEX2DEC(RIGHT(D2,2))*12-2)=LEN(F2),1,0)),(IF((HEX2DEC(RIGHT(D2,2))*12)=LEN(F2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I9">
-    <cfRule type="expression" dxfId="88" priority="5">
+    <cfRule type="expression" dxfId="224" priority="5">
       <formula>IF(HEX2DEC(RIGHT(E2,2))&gt;0,(IF((HEX2DEC(RIGHT(E2,2))*12-2)=LEN(H2),1,0)),(IF((HEX2DEC(RIGHT(E2,2))*12)=LEN(H2),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="87" priority="2">
+    <cfRule type="expression" dxfId="223" priority="2">
       <formula>IF(HEX2DEC(RIGHT(D9,2))&gt;0,(IF((HEX2DEC(RIGHT(D9,2))*12-2)=LEN(F9),1,0)),(IF((HEX2DEC(RIGHT(D9,2))*12)=LEN(F9),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="86" priority="1">
+    <cfRule type="expression" dxfId="222" priority="1">
       <formula>IF(HEX2DEC(RIGHT(E9,2))&gt;0,(IF((HEX2DEC(RIGHT(E9,2))*12-2)=LEN(H9),1,0)),(IF((HEX2DEC(RIGHT(E9,2))*12)=LEN(H9),1,0)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
#16: planter data mask changes.
</commit_message>
<xml_diff>
--- a/MapeamentoID_OP.xlsx
+++ b/MapeamentoID_OP.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qualicode\Documents\repos\M2GPlus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leandro\View0\M2GPlus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="833" firstSheet="7" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="833" firstSheet="9" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="ID'S" sheetId="1" r:id="rId1"/>
@@ -13670,7 +13670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -13867,6 +13867,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16098,7 +16099,7 @@
   <dimension ref="A1:AM24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="A21:B21"/>
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16725,7 +16726,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17312,8 +17313,8 @@
   <dimension ref="A1:P135"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B130" sqref="B130:L130"/>
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H120" sqref="H120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24483,7 +24484,7 @@
   <sheetPr codeName="Plan8"/>
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N5" sqref="A5:N5"/>
     </sheetView>
   </sheetViews>
@@ -25507,8 +25508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q325"/>
   <sheetViews>
-    <sheetView topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="C290" sqref="C290"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38249,7 +38250,7 @@
         <v>383</v>
       </c>
       <c r="F255" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G255" t="s">
         <v>25</v>
@@ -38299,7 +38300,7 @@
         <v>383</v>
       </c>
       <c r="F256" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G256" t="s">
         <v>25</v>
@@ -38349,7 +38350,7 @@
         <v>383</v>
       </c>
       <c r="F257" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G257" t="s">
         <v>25</v>
@@ -38399,7 +38400,7 @@
         <v>383</v>
       </c>
       <c r="F258" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G258" t="s">
         <v>25</v>
@@ -38449,7 +38450,7 @@
         <v>383</v>
       </c>
       <c r="F259" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G259" t="s">
         <v>25</v>
@@ -38499,7 +38500,7 @@
         <v>383</v>
       </c>
       <c r="F260" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G260" t="s">
         <v>25</v>
@@ -38549,7 +38550,7 @@
         <v>383</v>
       </c>
       <c r="F261" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G261" t="s">
         <v>25</v>
@@ -38599,7 +38600,7 @@
         <v>383</v>
       </c>
       <c r="F262" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G262" t="s">
         <v>25</v>
@@ -38649,7 +38650,7 @@
         <v>383</v>
       </c>
       <c r="F263" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G263" t="s">
         <v>25</v>
@@ -38699,7 +38700,7 @@
         <v>383</v>
       </c>
       <c r="F264" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G264" t="s">
         <v>25</v>
@@ -38749,7 +38750,7 @@
         <v>383</v>
       </c>
       <c r="F265" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G265" t="s">
         <v>25</v>
@@ -38799,7 +38800,7 @@
         <v>383</v>
       </c>
       <c r="F266" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G266" t="s">
         <v>25</v>
@@ -38849,7 +38850,7 @@
         <v>383</v>
       </c>
       <c r="F267" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G267" t="s">
         <v>25</v>
@@ -38899,7 +38900,7 @@
         <v>383</v>
       </c>
       <c r="F268" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G268" t="s">
         <v>25</v>
@@ -38949,7 +38950,7 @@
         <v>383</v>
       </c>
       <c r="F269" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G269" t="s">
         <v>25</v>
@@ -38999,7 +39000,7 @@
         <v>383</v>
       </c>
       <c r="F270" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G270" t="s">
         <v>25</v>
@@ -39049,7 +39050,7 @@
         <v>383</v>
       </c>
       <c r="F271" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G271" t="s">
         <v>25</v>
@@ -39099,7 +39100,7 @@
         <v>383</v>
       </c>
       <c r="F272" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G272" t="s">
         <v>25</v>
@@ -39149,7 +39150,7 @@
         <v>383</v>
       </c>
       <c r="F273" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G273" t="s">
         <v>25</v>
@@ -39199,7 +39200,7 @@
         <v>383</v>
       </c>
       <c r="F274" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G274" t="s">
         <v>25</v>
@@ -39249,7 +39250,7 @@
         <v>383</v>
       </c>
       <c r="F275" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G275" t="s">
         <v>25</v>
@@ -39299,7 +39300,7 @@
         <v>383</v>
       </c>
       <c r="F276" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G276" t="s">
         <v>25</v>
@@ -39349,7 +39350,7 @@
         <v>383</v>
       </c>
       <c r="F277" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G277" t="s">
         <v>25</v>
@@ -39399,7 +39400,7 @@
         <v>383</v>
       </c>
       <c r="F278" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G278" t="s">
         <v>25</v>
@@ -39449,7 +39450,7 @@
         <v>383</v>
       </c>
       <c r="F279" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G279" t="s">
         <v>25</v>
@@ -39499,7 +39500,7 @@
         <v>383</v>
       </c>
       <c r="F280" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G280" t="s">
         <v>25</v>
@@ -39549,7 +39550,7 @@
         <v>383</v>
       </c>
       <c r="F281" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G281" t="s">
         <v>25</v>
@@ -39599,7 +39600,7 @@
         <v>383</v>
       </c>
       <c r="F282" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G282" t="s">
         <v>25</v>
@@ -39649,7 +39650,7 @@
         <v>383</v>
       </c>
       <c r="F283" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G283" t="s">
         <v>25</v>
@@ -39699,7 +39700,7 @@
         <v>383</v>
       </c>
       <c r="F284" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G284" t="s">
         <v>25</v>
@@ -39749,7 +39750,7 @@
         <v>383</v>
       </c>
       <c r="F285" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G285" t="s">
         <v>25</v>
@@ -39799,7 +39800,7 @@
         <v>383</v>
       </c>
       <c r="F286" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G286" t="s">
         <v>25</v>
@@ -39849,7 +39850,7 @@
         <v>383</v>
       </c>
       <c r="F287" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G287" t="s">
         <v>25</v>
@@ -39899,7 +39900,7 @@
         <v>383</v>
       </c>
       <c r="F288" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G288" t="s">
         <v>25</v>
@@ -39949,7 +39950,7 @@
         <v>383</v>
       </c>
       <c r="F289" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G289" t="s">
         <v>25</v>
@@ -39983,7 +39984,7 @@
       </c>
     </row>
     <row r="290" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
+      <c r="A290" s="72" t="s">
         <v>1362</v>
       </c>
       <c r="B290" t="s">
@@ -39999,7 +40000,7 @@
         <v>383</v>
       </c>
       <c r="F290" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G290" t="s">
         <v>25</v>
@@ -40049,7 +40050,7 @@
         <v>383</v>
       </c>
       <c r="F291" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G291" t="s">
         <v>25</v>
@@ -40073,7 +40074,7 @@
         <v>23</v>
       </c>
       <c r="N291" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O291" t="s">
         <v>23</v>
@@ -40099,7 +40100,7 @@
         <v>383</v>
       </c>
       <c r="F292" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G292" t="s">
         <v>25</v>
@@ -40123,7 +40124,7 @@
         <v>23</v>
       </c>
       <c r="N292" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O292" t="s">
         <v>23</v>
@@ -40149,7 +40150,7 @@
         <v>383</v>
       </c>
       <c r="F293" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G293" t="s">
         <v>25</v>
@@ -40173,7 +40174,7 @@
         <v>23</v>
       </c>
       <c r="N293" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O293" t="s">
         <v>23</v>
@@ -40199,7 +40200,7 @@
         <v>383</v>
       </c>
       <c r="F294" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G294" t="s">
         <v>25</v>
@@ -40223,7 +40224,7 @@
         <v>23</v>
       </c>
       <c r="N294" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O294" t="s">
         <v>23</v>
@@ -40249,7 +40250,7 @@
         <v>383</v>
       </c>
       <c r="F295" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G295" t="s">
         <v>25</v>
@@ -40273,7 +40274,7 @@
         <v>23</v>
       </c>
       <c r="N295" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O295" t="s">
         <v>23</v>
@@ -40299,7 +40300,7 @@
         <v>383</v>
       </c>
       <c r="F296" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G296" t="s">
         <v>25</v>
@@ -40323,7 +40324,7 @@
         <v>23</v>
       </c>
       <c r="N296" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O296" t="s">
         <v>23</v>
@@ -40349,7 +40350,7 @@
         <v>383</v>
       </c>
       <c r="F297" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G297" t="s">
         <v>25</v>
@@ -40373,7 +40374,7 @@
         <v>23</v>
       </c>
       <c r="N297" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O297" t="s">
         <v>23</v>
@@ -40399,7 +40400,7 @@
         <v>383</v>
       </c>
       <c r="F298" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G298" t="s">
         <v>25</v>
@@ -40423,7 +40424,7 @@
         <v>23</v>
       </c>
       <c r="N298" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O298" t="s">
         <v>23</v>
@@ -40449,7 +40450,7 @@
         <v>383</v>
       </c>
       <c r="F299" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G299" t="s">
         <v>25</v>
@@ -40473,7 +40474,7 @@
         <v>23</v>
       </c>
       <c r="N299" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O299" t="s">
         <v>23</v>
@@ -40499,7 +40500,7 @@
         <v>383</v>
       </c>
       <c r="F300" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G300" t="s">
         <v>25</v>
@@ -40523,7 +40524,7 @@
         <v>23</v>
       </c>
       <c r="N300" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O300" t="s">
         <v>23</v>
@@ -40549,7 +40550,7 @@
         <v>383</v>
       </c>
       <c r="F301" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G301" t="s">
         <v>25</v>
@@ -40573,7 +40574,7 @@
         <v>23</v>
       </c>
       <c r="N301" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O301" t="s">
         <v>23</v>
@@ -40599,7 +40600,7 @@
         <v>383</v>
       </c>
       <c r="F302" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G302" t="s">
         <v>25</v>
@@ -40623,7 +40624,7 @@
         <v>23</v>
       </c>
       <c r="N302" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O302" t="s">
         <v>23</v>
@@ -40649,7 +40650,7 @@
         <v>383</v>
       </c>
       <c r="F303" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G303" t="s">
         <v>25</v>
@@ -40673,7 +40674,7 @@
         <v>23</v>
       </c>
       <c r="N303" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O303" t="s">
         <v>23</v>
@@ -40699,7 +40700,7 @@
         <v>383</v>
       </c>
       <c r="F304" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G304" t="s">
         <v>25</v>
@@ -40723,7 +40724,7 @@
         <v>23</v>
       </c>
       <c r="N304" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O304" t="s">
         <v>23</v>
@@ -40749,7 +40750,7 @@
         <v>383</v>
       </c>
       <c r="F305" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G305" t="s">
         <v>25</v>
@@ -40773,7 +40774,7 @@
         <v>23</v>
       </c>
       <c r="N305" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O305" t="s">
         <v>23</v>
@@ -40799,7 +40800,7 @@
         <v>383</v>
       </c>
       <c r="F306" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G306" t="s">
         <v>25</v>
@@ -40823,7 +40824,7 @@
         <v>23</v>
       </c>
       <c r="N306" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O306" t="s">
         <v>23</v>
@@ -40849,7 +40850,7 @@
         <v>383</v>
       </c>
       <c r="F307" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G307" t="s">
         <v>25</v>
@@ -40873,7 +40874,7 @@
         <v>23</v>
       </c>
       <c r="N307" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O307" t="s">
         <v>23</v>
@@ -40899,7 +40900,7 @@
         <v>383</v>
       </c>
       <c r="F308" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G308" t="s">
         <v>25</v>
@@ -40923,7 +40924,7 @@
         <v>23</v>
       </c>
       <c r="N308" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O308" t="s">
         <v>23</v>
@@ -40949,7 +40950,7 @@
         <v>383</v>
       </c>
       <c r="F309" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G309" t="s">
         <v>25</v>
@@ -40973,7 +40974,7 @@
         <v>23</v>
       </c>
       <c r="N309" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O309" t="s">
         <v>23</v>
@@ -40999,7 +41000,7 @@
         <v>383</v>
       </c>
       <c r="F310" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G310" t="s">
         <v>25</v>
@@ -41023,7 +41024,7 @@
         <v>23</v>
       </c>
       <c r="N310" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O310" t="s">
         <v>23</v>
@@ -41049,7 +41050,7 @@
         <v>383</v>
       </c>
       <c r="F311" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G311" t="s">
         <v>25</v>
@@ -41073,7 +41074,7 @@
         <v>23</v>
       </c>
       <c r="N311" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O311" t="s">
         <v>23</v>
@@ -41099,7 +41100,7 @@
         <v>383</v>
       </c>
       <c r="F312" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G312" t="s">
         <v>25</v>
@@ -41123,7 +41124,7 @@
         <v>23</v>
       </c>
       <c r="N312" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O312" t="s">
         <v>23</v>
@@ -41149,7 +41150,7 @@
         <v>383</v>
       </c>
       <c r="F313" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G313" t="s">
         <v>25</v>
@@ -41173,7 +41174,7 @@
         <v>23</v>
       </c>
       <c r="N313" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O313" t="s">
         <v>23</v>
@@ -41199,7 +41200,7 @@
         <v>383</v>
       </c>
       <c r="F314" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G314" t="s">
         <v>25</v>
@@ -41223,7 +41224,7 @@
         <v>23</v>
       </c>
       <c r="N314" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O314" t="s">
         <v>23</v>
@@ -41249,7 +41250,7 @@
         <v>383</v>
       </c>
       <c r="F315" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G315" t="s">
         <v>25</v>
@@ -41273,7 +41274,7 @@
         <v>23</v>
       </c>
       <c r="N315" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O315" t="s">
         <v>23</v>
@@ -41299,7 +41300,7 @@
         <v>383</v>
       </c>
       <c r="F316" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G316" t="s">
         <v>25</v>
@@ -41323,7 +41324,7 @@
         <v>23</v>
       </c>
       <c r="N316" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O316" t="s">
         <v>23</v>
@@ -41349,7 +41350,7 @@
         <v>383</v>
       </c>
       <c r="F317" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G317" t="s">
         <v>25</v>
@@ -41373,7 +41374,7 @@
         <v>23</v>
       </c>
       <c r="N317" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O317" t="s">
         <v>23</v>
@@ -41399,7 +41400,7 @@
         <v>383</v>
       </c>
       <c r="F318" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G318" t="s">
         <v>25</v>
@@ -41423,7 +41424,7 @@
         <v>23</v>
       </c>
       <c r="N318" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O318" t="s">
         <v>23</v>
@@ -41449,7 +41450,7 @@
         <v>383</v>
       </c>
       <c r="F319" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G319" t="s">
         <v>25</v>
@@ -41473,7 +41474,7 @@
         <v>23</v>
       </c>
       <c r="N319" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O319" t="s">
         <v>23</v>
@@ -41499,7 +41500,7 @@
         <v>383</v>
       </c>
       <c r="F320" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G320" t="s">
         <v>25</v>
@@ -41523,7 +41524,7 @@
         <v>23</v>
       </c>
       <c r="N320" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O320" t="s">
         <v>23</v>
@@ -41549,7 +41550,7 @@
         <v>383</v>
       </c>
       <c r="F321" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G321" t="s">
         <v>25</v>
@@ -41573,7 +41574,7 @@
         <v>23</v>
       </c>
       <c r="N321" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O321" t="s">
         <v>23</v>
@@ -41599,7 +41600,7 @@
         <v>383</v>
       </c>
       <c r="F322" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G322" t="s">
         <v>25</v>
@@ -41623,7 +41624,7 @@
         <v>23</v>
       </c>
       <c r="N322" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O322" t="s">
         <v>23</v>
@@ -41649,7 +41650,7 @@
         <v>383</v>
       </c>
       <c r="F323" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G323" t="s">
         <v>25</v>
@@ -41673,7 +41674,7 @@
         <v>23</v>
       </c>
       <c r="N323" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O323" t="s">
         <v>23</v>
@@ -41699,7 +41700,7 @@
         <v>383</v>
       </c>
       <c r="F324" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G324" t="s">
         <v>25</v>
@@ -41723,7 +41724,7 @@
         <v>23</v>
       </c>
       <c r="N324" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O324" t="s">
         <v>23</v>
@@ -41749,7 +41750,7 @@
         <v>383</v>
       </c>
       <c r="F325" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G325" t="s">
         <v>25</v>
@@ -41773,7 +41774,7 @@
         <v>23</v>
       </c>
       <c r="N325" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="O325" t="s">
         <v>23</v>
@@ -41784,8 +41785,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -49239,8 +49241,8 @@
   <sheetPr codeName="Plan12"/>
   <dimension ref="A1:E483"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D483" sqref="D483"/>
     </sheetView>
   </sheetViews>
@@ -69471,8 +69473,8 @@
   <sheetPr codeName="Plan13"/>
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56:F57"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -71340,7 +71342,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -77956,7 +77958,9 @@
   <sheetPr codeName="Plan4"/>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
#18: Update isobus id map doc file
</commit_message>
<xml_diff>
--- a/MapeamentoID_OP.xlsx
+++ b/MapeamentoID_OP.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leandro\View0\M2GPlus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Leandro\View0\M2GPlus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="833" firstSheet="9" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="833" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ID'S" sheetId="1" r:id="rId1"/>
@@ -17313,8 +17313,8 @@
   <dimension ref="A1:P135"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H120" sqref="H120"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21700,9 +21700,9 @@
   <sheetPr codeName="Plan7"/>
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T53" sqref="T53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41798,8 +41798,8 @@
   <dimension ref="A1:R145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R74" sqref="A74:R74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49241,8 +49241,8 @@
   <sheetPr codeName="Plan12"/>
   <dimension ref="A1:E483"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A362" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D483" sqref="D483"/>
     </sheetView>
   </sheetViews>
@@ -69473,8 +69473,8 @@
   <sheetPr codeName="Plan13"/>
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:F102"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -71340,9 +71340,9 @@
   <sheetPr codeName="Plan3"/>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>